<commit_message>
Finished updating the name files (_example for all example files)
</commit_message>
<xml_diff>
--- a/Excel_References_Example.xlsx
+++ b/Excel_References_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/ennowinkler_ennosgermancourse_onmicrosoft_com/Documents/excelbib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E0322B3-2A80-4E64-AB8A-D113095508BE}"/>
+  <xr:revisionPtr revIDLastSave="233" documentId="13_ncr:1_{92D5FB84-227A-4306-9187-93183921DEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{380E0EB2-5ED8-4583-98A3-9CDB88807129}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1890" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1890" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="30" r:id="rId1"/>
@@ -110,18 +110,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>@article{test2024,
-  title = {A sample article},
-  volume = {16},
-  journal = {Awesome Journal},
-  publisher = {Awesome Publisher},
-  author = {Doe,  Kim},
-  year = {2024},
-  month = aug,
-  pages = {154–158}
-}</t>
   </si>
   <si>
     <t>Bibtex templates</t>
@@ -522,6 +510,18 @@
 If you have a doi, you can add the "doi" field like in the green field below. DON'T add "https://doi.org/" before the DOI, Rmarkdown will write it for you. 
 However, most DOI links can be converted into Bibtex easily so you won't have to write them by hand. 
 I use doi2bib.org, but any bib generator works. </t>
+  </si>
+  <si>
+    <t>@article{test2024,
+  title = {A sample article},
+  volume = {16},
+  journal = {Journal of Examples},
+  publisher = {Example Publisher},
+  author = {Doe,  Kim},
+  year = {2024},
+  month = aug,
+  pages = {154–158}
+}</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E656E9-B3BA-44E1-9F7B-B05F659FF79F}">
   <dimension ref="A1:I507"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -17257,10 +17257,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R508"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B5" sqref="B5"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -17341,7 +17341,7 @@
     </row>
     <row r="2" spans="1:18" ht="150" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="26" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="B2" s="15" t="str">
         <f>IFERROR("@" &amp; MID(A2, SEARCH("{", A2) + 1, SEARCH(",", A2) - SEARCH("{", A2) - 1), "")</f>
@@ -33534,176 +33534,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="28"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>